<commit_message>
Commiting the latest changes
</commit_message>
<xml_diff>
--- a/Solina/Production/Input.xlsx
+++ b/Solina/Production/Input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>Data</t>
   </si>
@@ -32,63 +32,6 @@
   </si>
   <si>
     <t>Lookup</t>
-  </si>
-  <si>
-    <t>14.02.202415</t>
-  </si>
-  <si>
-    <t>14.02.202416</t>
-  </si>
-  <si>
-    <t>14.02.202417</t>
-  </si>
-  <si>
-    <t>14.02.202418</t>
-  </si>
-  <si>
-    <t>14.02.202419</t>
-  </si>
-  <si>
-    <t>14.02.202420</t>
-  </si>
-  <si>
-    <t>14.02.202421</t>
-  </si>
-  <si>
-    <t>14.02.202422</t>
-  </si>
-  <si>
-    <t>14.02.202423</t>
-  </si>
-  <si>
-    <t>15.02.20240</t>
-  </si>
-  <si>
-    <t>15.02.20241</t>
-  </si>
-  <si>
-    <t>15.02.20242</t>
-  </si>
-  <si>
-    <t>15.02.20243</t>
-  </si>
-  <si>
-    <t>15.02.20244</t>
-  </si>
-  <si>
-    <t>15.02.20245</t>
-  </si>
-  <si>
-    <t>15.02.20246</t>
-  </si>
-  <si>
-    <t>15.02.20247</t>
-  </si>
-  <si>
-    <t>15.02.20248</t>
-  </si>
-  <si>
-    <t>15.02.20249</t>
   </si>
   <si>
     <t>15.02.202410</t>
@@ -709,19 +652,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>103.08</v>
+        <v>384.43</v>
       </c>
       <c r="D2">
-        <v>7.36</v>
+        <v>7.06</v>
       </c>
       <c r="E2">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -729,19 +672,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>52.4</v>
+        <v>471.14</v>
       </c>
       <c r="D3">
-        <v>7.07</v>
+        <v>7.23</v>
       </c>
       <c r="E3">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -749,19 +692,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>9.08</v>
+        <v>507.42</v>
       </c>
       <c r="D4">
-        <v>6.79</v>
+        <v>7.6</v>
       </c>
       <c r="E4">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -769,19 +712,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>489.3</v>
       </c>
       <c r="D5">
-        <v>6.41</v>
+        <v>7.96</v>
       </c>
       <c r="E5">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -789,19 +732,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>418.76</v>
       </c>
       <c r="D6">
-        <v>5.88</v>
+        <v>8.16</v>
       </c>
       <c r="E6">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -809,19 +752,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>303.9</v>
       </c>
       <c r="D7">
-        <v>4.97</v>
+        <v>7.83</v>
       </c>
       <c r="E7">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -829,19 +772,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>160.51</v>
       </c>
       <c r="D8">
-        <v>4.52</v>
+        <v>6.11</v>
       </c>
       <c r="E8">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -849,19 +792,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>28.17</v>
       </c>
       <c r="D9">
-        <v>4.11</v>
+        <v>5.53</v>
       </c>
       <c r="E9">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -869,19 +812,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3.68</v>
+        <v>5.12</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -892,16 +835,16 @@
         <v>45337</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3.13</v>
+        <v>4.74</v>
       </c>
       <c r="E11">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -912,16 +855,16 @@
         <v>45337</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>2.64</v>
+        <v>4.38</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -932,16 +875,16 @@
         <v>45337</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>2.24</v>
+        <v>4.04</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -952,16 +895,16 @@
         <v>45337</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1.92</v>
+        <v>3.72</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -972,16 +915,16 @@
         <v>45337</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1.66</v>
+        <v>3.41</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -989,19 +932,19 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1.49</v>
+        <v>3.13</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
@@ -1009,19 +952,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1.71</v>
+        <v>2.84</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
@@ -1029,19 +972,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>7.03</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>3.14</v>
+        <v>2.55</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -1049,19 +992,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>110.65</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>4.52</v>
+        <v>2.32</v>
       </c>
       <c r="E19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1069,19 +1012,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>257.67</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>5.73</v>
+        <v>2.16</v>
       </c>
       <c r="E20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1089,19 +1032,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>384.43</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>6.92</v>
+        <v>2.04</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -1109,19 +1052,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>471.14</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>7.87</v>
+        <v>2.29</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
@@ -1129,19 +1072,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>507.42</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="D23">
-        <v>8.42</v>
+        <v>3.89</v>
       </c>
       <c r="E23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
@@ -1149,16 +1092,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>489.3</v>
+        <v>115.07</v>
       </c>
       <c r="D24">
-        <v>8.609999999999999</v>
+        <v>5.45</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -1169,16 +1112,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>418.76</v>
+        <v>262.96</v>
       </c>
       <c r="D25">
-        <v>8.48</v>
+        <v>6.79</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1189,16 +1132,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>303.9</v>
+        <v>390.13</v>
       </c>
       <c r="D26">
-        <v>7.71</v>
+        <v>7.97</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1209,16 +1152,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>160.51</v>
+        <v>477.02</v>
       </c>
       <c r="D27">
-        <v>5.93</v>
+        <v>8.9</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1229,16 +1172,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>28.17</v>
+        <v>513.35</v>
       </c>
       <c r="D28">
-        <v>5.34</v>
+        <v>9.59</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1249,19 +1192,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B29">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>495.14</v>
       </c>
       <c r="D29">
-        <v>4.93</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -1269,16 +1212,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B30">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>424.38</v>
       </c>
       <c r="D30">
-        <v>4.53</v>
+        <v>9.92</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1289,19 +1232,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>309.12</v>
       </c>
       <c r="D31">
-        <v>4.15</v>
+        <v>8.93</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
@@ -1309,16 +1252,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B32">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>165.07</v>
       </c>
       <c r="D32">
-        <v>3.81</v>
+        <v>7.04</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1329,19 +1272,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B33">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>30.47</v>
       </c>
       <c r="D33">
-        <v>3.47</v>
+        <v>6.39</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
@@ -1349,19 +1292,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>3.16</v>
+        <v>5.92</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
@@ -1372,16 +1315,16 @@
         <v>45338</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>2.86</v>
+        <v>5.55</v>
       </c>
       <c r="E35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -1392,16 +1335,16 @@
         <v>45338</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>2.55</v>
+        <v>5.22</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -1412,16 +1355,16 @@
         <v>45338</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>2.3</v>
+        <v>4.9</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
@@ -1432,16 +1375,16 @@
         <v>45338</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>2.08</v>
+        <v>4.6</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
@@ -1452,16 +1395,16 @@
         <v>45338</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>1.93</v>
+        <v>4.29</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
@@ -1469,19 +1412,19 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>1.86</v>
+        <v>3.99</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
@@ -1489,19 +1432,19 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>2.11</v>
+        <v>3.72</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F41" t="s">
         <v>45</v>
@@ -1509,19 +1452,19 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>8.210000000000001</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>3.69</v>
+        <v>3.5</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" t="s">
         <v>46</v>
@@ -1529,19 +1472,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>115.07</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>5.19</v>
+        <v>3.21</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -1549,19 +1492,19 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>262.96</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>6.47</v>
+        <v>3.01</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
@@ -1569,19 +1512,19 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>390.13</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>7.68</v>
+        <v>2.84</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
@@ -1589,19 +1532,19 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>477.02</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>8.6</v>
+        <v>3.14</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
@@ -1609,16 +1552,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>513.34</v>
+        <v>9.49</v>
       </c>
       <c r="D47">
-        <v>9.27</v>
+        <v>4.94</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1629,16 +1572,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>495.14</v>
+        <v>119.58</v>
       </c>
       <c r="D48">
-        <v>9.640000000000001</v>
+        <v>6.56</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1649,16 +1592,16 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>424.37</v>
+        <v>268.31</v>
       </c>
       <c r="D49">
-        <v>9.619999999999999</v>
+        <v>8.1</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1678,13 +1621,13 @@
         <v>309.12</v>
       </c>
       <c r="D50">
-        <v>8.529999999999999</v>
+        <v>8.93</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1695,16 +1638,16 @@
         <v>16</v>
       </c>
       <c r="C51">
-        <v>165.06</v>
+        <v>165.07</v>
       </c>
       <c r="D51">
-        <v>6.61</v>
+        <v>7.04</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1718,13 +1661,13 @@
         <v>30.47</v>
       </c>
       <c r="D52">
-        <v>5.95</v>
+        <v>6.39</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1738,13 +1681,13 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>5.47</v>
+        <v>5.92</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1758,13 +1701,13 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <v>5.1</v>
+        <v>5.55</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1778,13 +1721,13 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>4.76</v>
+        <v>5.22</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1798,13 +1741,13 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <v>4.45</v>
+        <v>4.9</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1818,13 +1761,13 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>4.14</v>
+        <v>4.6</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1838,13 +1781,13 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <v>3.82</v>
+        <v>4.29</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1858,13 +1801,13 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>3.53</v>
+        <v>3.99</v>
       </c>
       <c r="E59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1878,13 +1821,13 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>3.23</v>
+        <v>3.72</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F60" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1898,13 +1841,13 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>2.97</v>
+        <v>3.5</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1918,13 +1861,13 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <v>2.76</v>
+        <v>3.21</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1938,13 +1881,13 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>2.52</v>
+        <v>3.01</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1958,13 +1901,13 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <v>2.43</v>
+        <v>2.84</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1978,13 +1921,13 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>2.79</v>
+        <v>3.14</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1998,13 +1941,13 @@
         <v>9.49</v>
       </c>
       <c r="D66">
-        <v>4.59</v>
+        <v>4.94</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2015,16 +1958,16 @@
         <v>8</v>
       </c>
       <c r="C67">
-        <v>119.56</v>
+        <v>119.58</v>
       </c>
       <c r="D67">
-        <v>6.37</v>
+        <v>6.56</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2035,16 +1978,16 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>268.3</v>
+        <v>268.31</v>
       </c>
       <c r="D68">
-        <v>8.039999999999999</v>
+        <v>8.1</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2055,16 +1998,10 @@
         <v>10</v>
       </c>
       <c r="C69">
-        <v>395.85</v>
-      </c>
-      <c r="D69">
-        <v>9.41</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
+        <v>395.86</v>
       </c>
       <c r="F69" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2077,14 +2014,8 @@
       <c r="C70">
         <v>482.93</v>
       </c>
-      <c r="D70">
-        <v>10.53</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
       <c r="F70" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2097,14 +2028,8 @@
       <c r="C71">
         <v>519.29</v>
       </c>
-      <c r="D71">
-        <v>11.35</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
       <c r="F71" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2115,16 +2040,10 @@
         <v>13</v>
       </c>
       <c r="C72">
-        <v>500.99</v>
-      </c>
-      <c r="D72">
-        <v>11.73</v>
-      </c>
-      <c r="E72">
-        <v>6</v>
+        <v>500.98</v>
       </c>
       <c r="F72" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2137,14 +2056,8 @@
       <c r="C73">
         <v>429.98</v>
       </c>
-      <c r="D73">
-        <v>11.49</v>
-      </c>
-      <c r="E73">
-        <v>7</v>
-      </c>
       <c r="F73" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2157,14 +2070,8 @@
       <c r="C74">
         <v>314.32</v>
       </c>
-      <c r="D74">
-        <v>9.970000000000001</v>
-      </c>
-      <c r="E74">
-        <v>8</v>
-      </c>
       <c r="F74" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2175,16 +2082,10 @@
         <v>16</v>
       </c>
       <c r="C75">
-        <v>169.61</v>
-      </c>
-      <c r="D75">
-        <v>7.9</v>
-      </c>
-      <c r="E75">
-        <v>25</v>
+        <v>169.49</v>
       </c>
       <c r="F75" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2195,16 +2096,10 @@
         <v>17</v>
       </c>
       <c r="C76">
-        <v>32.81</v>
-      </c>
-      <c r="D76">
-        <v>7.27</v>
-      </c>
-      <c r="E76">
-        <v>36</v>
+        <v>32.6</v>
       </c>
       <c r="F76" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2217,14 +2112,8 @@
       <c r="C77">
         <v>0</v>
       </c>
-      <c r="D77">
-        <v>6.97</v>
-      </c>
-      <c r="E77">
-        <v>47</v>
-      </c>
       <c r="F77" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2237,14 +2126,8 @@
       <c r="C78">
         <v>0</v>
       </c>
-      <c r="D78">
-        <v>6.87</v>
-      </c>
-      <c r="E78">
-        <v>100</v>
-      </c>
       <c r="F78" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2257,14 +2140,8 @@
       <c r="C79">
         <v>0</v>
       </c>
-      <c r="D79">
-        <v>7.07</v>
-      </c>
-      <c r="E79">
-        <v>100</v>
-      </c>
       <c r="F79" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2277,14 +2154,8 @@
       <c r="C80">
         <v>0</v>
       </c>
-      <c r="D80">
-        <v>7.16</v>
-      </c>
-      <c r="E80">
-        <v>100</v>
-      </c>
       <c r="F80" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2297,14 +2168,8 @@
       <c r="C81">
         <v>0</v>
       </c>
-      <c r="D81">
-        <v>7.04</v>
-      </c>
-      <c r="E81">
-        <v>100</v>
-      </c>
       <c r="F81" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2317,14 +2182,8 @@
       <c r="C82">
         <v>0</v>
       </c>
-      <c r="D82">
-        <v>7.01</v>
-      </c>
-      <c r="E82">
-        <v>100</v>
-      </c>
       <c r="F82" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2337,14 +2196,8 @@
       <c r="C83">
         <v>0</v>
       </c>
-      <c r="D83">
-        <v>6.75</v>
-      </c>
-      <c r="E83">
-        <v>100</v>
-      </c>
       <c r="F83" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2357,14 +2210,8 @@
       <c r="C84">
         <v>0</v>
       </c>
-      <c r="D84">
-        <v>6.45</v>
-      </c>
-      <c r="E84">
-        <v>100</v>
-      </c>
       <c r="F84" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2377,14 +2224,8 @@
       <c r="C85">
         <v>0</v>
       </c>
-      <c r="D85">
-        <v>6.39</v>
-      </c>
-      <c r="E85">
-        <v>100</v>
-      </c>
       <c r="F85" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2397,14 +2238,8 @@
       <c r="C86">
         <v>0</v>
       </c>
-      <c r="D86">
-        <v>6.29</v>
-      </c>
-      <c r="E86">
-        <v>100</v>
-      </c>
       <c r="F86" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2417,14 +2252,8 @@
       <c r="C87">
         <v>0</v>
       </c>
-      <c r="D87">
-        <v>6.23</v>
-      </c>
-      <c r="E87">
-        <v>100</v>
-      </c>
       <c r="F87" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2437,14 +2266,8 @@
       <c r="C88">
         <v>0</v>
       </c>
-      <c r="D88">
-        <v>6.17</v>
-      </c>
-      <c r="E88">
-        <v>100</v>
-      </c>
       <c r="F88" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2457,14 +2280,8 @@
       <c r="C89">
         <v>0</v>
       </c>
-      <c r="D89">
-        <v>6.14</v>
-      </c>
-      <c r="E89">
-        <v>99</v>
-      </c>
       <c r="F89" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2477,14 +2294,8 @@
       <c r="C90">
         <v>2.95</v>
       </c>
-      <c r="D90">
-        <v>6.68</v>
-      </c>
-      <c r="E90">
-        <v>93</v>
-      </c>
       <c r="F90" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2497,14 +2308,8 @@
       <c r="C91">
         <v>42.95</v>
       </c>
-      <c r="D91">
-        <v>7.06</v>
-      </c>
-      <c r="E91">
-        <v>96</v>
-      </c>
       <c r="F91" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2517,14 +2322,8 @@
       <c r="C92">
         <v>104.98</v>
       </c>
-      <c r="D92">
-        <v>7.67</v>
-      </c>
-      <c r="E92">
-        <v>98</v>
-      </c>
       <c r="F92" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2537,14 +2336,8 @@
       <c r="C93">
         <v>130.85</v>
       </c>
-      <c r="D93">
-        <v>8.550000000000001</v>
-      </c>
-      <c r="E93">
-        <v>96</v>
-      </c>
       <c r="F93" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2557,14 +2350,8 @@
       <c r="C94">
         <v>158.28</v>
       </c>
-      <c r="D94">
-        <v>9.210000000000001</v>
-      </c>
-      <c r="E94">
-        <v>95</v>
-      </c>
       <c r="F94" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2577,14 +2364,8 @@
       <c r="C95">
         <v>185.98</v>
       </c>
-      <c r="D95">
-        <v>9.539999999999999</v>
-      </c>
-      <c r="E95">
-        <v>95</v>
-      </c>
       <c r="F95" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2597,14 +2378,8 @@
       <c r="C96">
         <v>185.31</v>
       </c>
-      <c r="D96">
-        <v>9.52</v>
-      </c>
-      <c r="E96">
-        <v>91</v>
-      </c>
       <c r="F96" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2617,14 +2392,8 @@
       <c r="C97">
         <v>172.41</v>
       </c>
-      <c r="D97">
-        <v>8.970000000000001</v>
-      </c>
-      <c r="E97">
-        <v>96</v>
-      </c>
       <c r="F97" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>